<commit_message>
Update helperland database schema.xlsx
</commit_message>
<xml_diff>
--- a/database/helperland database schema.xlsx
+++ b/database/helperland database schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ddcd2b4a77dd361/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ankit\helperland\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C02BEB6E-6944-4E86-BCFE-7AAC1B3B2008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128BA504-BF96-49EB-B26E-DD4C3B8C2F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9FA9E24-731D-4CBA-B3BA-DD830F3BCB7A}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>Service Provider</t>
   </si>
   <si>
-    <t>Service_provider_id</t>
-  </si>
-  <si>
     <t>Firstname</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Admin_id</t>
-  </si>
-  <si>
     <t>Service_provider_ID (Foregin key from service provider)</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
     <t>Customer Address</t>
   </si>
   <si>
-    <t>Address_ID</t>
-  </si>
-  <si>
     <t>House</t>
   </si>
   <si>
@@ -148,9 +139,6 @@
     <t>Service Request</t>
   </si>
   <si>
-    <t>Service_ID(Primary key)</t>
-  </si>
-  <si>
     <t>Customer_ID(Foregin key from customer)</t>
   </si>
   <si>
@@ -187,30 +175,18 @@
     <t>Status (Foreginkey from status)</t>
   </si>
   <si>
-    <t>ID(Primary)</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Rating</t>
   </si>
   <si>
-    <t>Rating_ID</t>
-  </si>
-  <si>
     <t>Service_provider_ID(Foregin key from service provider)</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
-    <t>Favourite_id</t>
-  </si>
-  <si>
-    <t>Customer_id(Primary Key)</t>
-  </si>
-  <si>
     <t>house_no</t>
   </si>
   <si>
@@ -221,6 +197,30 @@
   </si>
   <si>
     <t>Favourite</t>
+  </si>
+  <si>
+    <t>Customer_id(Primary Key &amp; Auto increment)</t>
+  </si>
+  <si>
+    <t>Service_provider_id(Primary Key &amp; Auto increment)</t>
+  </si>
+  <si>
+    <t>Address_ID(Primary Key &amp; Auto increment)</t>
+  </si>
+  <si>
+    <t>Service_ID(Primary Key &amp; Auto increment)</t>
+  </si>
+  <si>
+    <t>ID(Primary Key &amp; Auto increment)</t>
+  </si>
+  <si>
+    <t>Rating_ID(Primary Key &amp; Auto increment)</t>
+  </si>
+  <si>
+    <t>Favourite_id(Primary Key &amp; Auto increment)</t>
+  </si>
+  <si>
+    <t>Admin_id(Primary Key &amp; Auto increment)</t>
   </si>
 </sst>
 </file>
@@ -768,13 +768,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -786,22 +798,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3473DD1D-0818-496F-ADBC-BA3CEB65583A}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1160,11 +1160,11 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
@@ -1178,7 +1178,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="32"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="32"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="32"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="32"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
@@ -1272,7 +1272,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1304,11 +1304,11 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>6</v>
@@ -1322,26 +1322,26 @@
       <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="37"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4">
+        <v>100</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="40"/>
+      <c r="B15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4">
-        <v>100</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37"/>
-      <c r="B15" s="18" t="s">
-        <v>20</v>
-      </c>
       <c r="C15" s="28" t="s">
         <v>9</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="37"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="23" t="s">
         <v>11</v>
       </c>
@@ -1370,7 +1370,7 @@
       <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
@@ -1386,9 +1386,9 @@
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>14</v>
@@ -1400,9 +1400,9 @@
       <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="37"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>9</v>
@@ -1416,9 +1416,9 @@
       <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="37"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>9</v>
@@ -1432,9 +1432,9 @@
       <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="37"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>6</v>
@@ -1448,9 +1448,9 @@
       <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="37"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="25" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
@@ -1459,14 +1459,14 @@
         <v>10</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="37"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>9</v>
@@ -1475,14 +1475,14 @@
         <v>50</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="37"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="25" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>6</v>
@@ -1496,9 +1496,9 @@
       <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="37"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>9</v>
@@ -1512,12 +1512,12 @@
       <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="37"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="15" t="s">
@@ -1526,7 +1526,7 @@
       <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="26" t="s">
         <v>16</v>
       </c>
@@ -1542,9 +1542,9 @@
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="38"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>6</v>
@@ -1569,11 +1569,11 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="30" t="s">
-        <v>32</v>
+      <c r="A31" s="33" t="s">
+        <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>6</v>
@@ -1587,9 +1587,9 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="32"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>6</v>
@@ -1603,9 +1603,9 @@
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="32"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -1619,9 +1619,9 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="32"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -1635,9 +1635,9 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="32"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>6</v>
@@ -1651,9 +1651,9 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="32"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -1667,7 +1667,7 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="31"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="4" t="s">
         <v>12</v>
       </c>
@@ -1699,11 +1699,11 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="41" t="s">
-        <v>37</v>
+      <c r="A40" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>6</v>
@@ -1717,9 +1717,9 @@
       <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="32"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>6</v>
@@ -1733,9 +1733,9 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="32"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>6</v>
@@ -1744,14 +1744,14 @@
         <v>100</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="32"/>
+      <c r="A43" s="34"/>
       <c r="B43" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>14</v>
@@ -1763,12 +1763,12 @@
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="32"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
@@ -1777,12 +1777,12 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="32"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
@@ -1791,9 +1791,9 @@
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="32"/>
+      <c r="A46" s="34"/>
       <c r="B46" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
@@ -1807,9 +1807,9 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="32"/>
+      <c r="A47" s="34"/>
       <c r="B47" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -1823,12 +1823,12 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="32"/>
+      <c r="A48" s="34"/>
       <c r="B48" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
@@ -1837,12 +1837,12 @@
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="32"/>
+      <c r="A49" s="34"/>
       <c r="B49" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D49" s="4">
         <v>100</v>
@@ -1853,9 +1853,9 @@
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="32"/>
+      <c r="A50" s="34"/>
       <c r="B50" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
@@ -1869,9 +1869,9 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="31"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
@@ -1901,11 +1901,11 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="30" t="s">
-        <v>26</v>
+      <c r="A54" s="33" t="s">
+        <v>25</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>6</v>
@@ -1919,9 +1919,9 @@
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="31"/>
+      <c r="A55" s="35"/>
       <c r="B55" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
@@ -1951,11 +1951,11 @@
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="30" t="s">
-        <v>53</v>
+      <c r="A58" s="33" t="s">
+        <v>48</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>6</v>
@@ -1969,9 +1969,9 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="32"/>
+      <c r="A59" s="34"/>
       <c r="B59" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>6</v>
@@ -1985,9 +1985,9 @@
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="32"/>
+      <c r="A60" s="34"/>
       <c r="B60" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>6</v>
@@ -2001,12 +2001,12 @@
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="32"/>
+      <c r="A61" s="34"/>
       <c r="B61" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D61" s="4">
         <v>10</v>
@@ -2017,9 +2017,9 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="31"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>9</v>
@@ -2049,11 +2049,11 @@
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="33" t="s">
-        <v>62</v>
+      <c r="A65" s="37" t="s">
+        <v>54</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>6</v>
@@ -2062,14 +2062,14 @@
         <v>100</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="34"/>
+      <c r="A66" s="38"/>
       <c r="B66" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>6</v>
@@ -2078,14 +2078,14 @@
         <v>100</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="35"/>
+      <c r="A67" s="39"/>
       <c r="B67" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>6</v>
@@ -2094,7 +2094,7 @@
         <v>100</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F67" s="3"/>
     </row>
@@ -2108,11 +2108,11 @@
     </row>
     <row r="69" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="70" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="36" t="s">
-        <v>28</v>
+      <c r="A70" s="30" t="s">
+        <v>27</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>6</v>
@@ -2125,9 +2125,9 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="39"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>9</v>
@@ -2140,7 +2140,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="39"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="4" t="s">
         <v>11</v>
       </c>
@@ -2155,7 +2155,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="40"/>
+      <c r="A73" s="32"/>
       <c r="B73" s="12" t="s">
         <v>16</v>
       </c>
@@ -2174,14 +2174,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A13:A28"/>
+    <mergeCell ref="A3:A10"/>
     <mergeCell ref="A70:A73"/>
     <mergeCell ref="A31:A37"/>
     <mergeCell ref="A40:A51"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A58:A62"/>
     <mergeCell ref="A65:A67"/>
-    <mergeCell ref="A13:A28"/>
-    <mergeCell ref="A3:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2189,21 +2189,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC1F3D3FB021D45B765D6987C4FC9D1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9676eabfacdc1b957fbc60fea748797e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0b096726-50b8-4c0d-917f-c544d6902965" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a8fd738069329283a4013292edf0a54" ns3:_="">
     <xsd:import namespace="0b096726-50b8-4c0d-917f-c544d6902965"/>
@@ -2335,31 +2320,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED68C9C1-E095-41A2-9BD7-CE1753381607}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="0b096726-50b8-4c0d-917f-c544d6902965"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3D5A970-3B9D-48CF-B9E9-B1A4EA9FF8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88F85A4A-1B6B-44B4-9E94-5FAD513CB6CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2375,4 +2351,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3D5A970-3B9D-48CF-B9E9-B1A4EA9FF8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED68C9C1-E095-41A2-9BD7-CE1753381607}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0b096726-50b8-4c0d-917f-c544d6902965"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>